<commit_message>
Get nicely formatted data for stats including transfer learning
</commit_message>
<xml_diff>
--- a/Analysis/subject_demographics.xlsx
+++ b/Analysis/subject_demographics.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F081821-B2BF-407B-9B27-F4A894344B3B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB4326F6-2AA8-4E5B-9BA6-CA0C03A04F58}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7002" yWindow="-336" windowWidth="17280" windowHeight="8994" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12630" yWindow="6678" windowWidth="17280" windowHeight="8994" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="42">
   <si>
     <t>Subject ID</t>
   </si>
@@ -58,9 +58,6 @@
     <t>Cap Size</t>
   </si>
   <si>
-    <t>useBehavioral</t>
-  </si>
-  <si>
     <t>b12a46</t>
   </si>
   <si>
@@ -152,6 +149,9 @@
   </si>
   <si>
     <t>MLL</t>
+  </si>
+  <si>
+    <t>Study Number</t>
   </si>
 </sst>
 </file>
@@ -473,8 +473,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -499,7 +499,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -526,18 +526,18 @@
         <v>9</v>
       </c>
       <c r="L1" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D2" s="2">
         <v>0</v>
@@ -549,33 +549,33 @@
         <v>15</v>
       </c>
       <c r="G2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I2" s="2">
         <v>21</v>
       </c>
       <c r="J2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K2" t="s">
-        <v>36</v>
-      </c>
-      <c r="L2" t="s">
-        <v>37</v>
+        <v>35</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D3" s="2">
         <v>0</v>
@@ -587,33 +587,33 @@
         <v>12</v>
       </c>
       <c r="G3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I3" s="2">
         <v>21</v>
       </c>
       <c r="J3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K3" t="s">
-        <v>36</v>
-      </c>
-      <c r="L3" t="s">
-        <v>37</v>
+        <v>35</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D4" s="2">
         <v>0</v>
@@ -625,33 +625,33 @@
         <v>14</v>
       </c>
       <c r="G4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I4" s="2">
         <v>29</v>
       </c>
       <c r="J4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K4" t="s">
-        <v>40</v>
-      </c>
-      <c r="L4" t="s">
-        <v>37</v>
+        <v>39</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D5" s="2">
         <v>0</v>
@@ -663,33 +663,33 @@
         <v>12</v>
       </c>
       <c r="G5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I5" s="2">
         <v>20</v>
       </c>
       <c r="J5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K5" t="s">
-        <v>36</v>
-      </c>
-      <c r="L5" t="s">
-        <v>37</v>
+        <v>35</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6">
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D6" s="2">
         <v>0</v>
@@ -701,33 +701,33 @@
         <v>21</v>
       </c>
       <c r="G6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I6" s="2">
         <v>20</v>
       </c>
       <c r="J6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K6" t="s">
-        <v>36</v>
-      </c>
-      <c r="L6" t="s">
-        <v>37</v>
+        <v>35</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7">
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D7" s="2">
         <v>0</v>
@@ -739,33 +739,33 @@
         <v>7</v>
       </c>
       <c r="G7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I7" s="2">
         <v>21</v>
       </c>
       <c r="J7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K7" t="s">
-        <v>40</v>
-      </c>
-      <c r="L7" t="s">
-        <v>37</v>
+        <v>39</v>
+      </c>
+      <c r="L7">
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8">
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D8" s="2">
         <v>0</v>
@@ -777,33 +777,33 @@
         <v>16</v>
       </c>
       <c r="G8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I8" s="2">
         <v>20</v>
       </c>
       <c r="J8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K8" t="s">
-        <v>40</v>
-      </c>
-      <c r="L8" t="s">
-        <v>37</v>
+        <v>39</v>
+      </c>
+      <c r="L8">
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9">
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D9" s="2">
         <v>0</v>
@@ -815,33 +815,33 @@
         <v>22</v>
       </c>
       <c r="G9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I9" s="2">
         <v>19</v>
       </c>
       <c r="J9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K9" t="s">
-        <v>36</v>
-      </c>
-      <c r="L9" t="s">
-        <v>37</v>
+        <v>35</v>
+      </c>
+      <c r="L9">
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D10" s="2">
         <v>0</v>
@@ -853,33 +853,33 @@
         <v>17</v>
       </c>
       <c r="G10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I10" s="2">
         <v>23</v>
       </c>
       <c r="J10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K10" t="s">
-        <v>36</v>
-      </c>
-      <c r="L10" t="s">
-        <v>37</v>
+        <v>35</v>
+      </c>
+      <c r="L10">
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D11" s="2">
         <v>0</v>
@@ -891,33 +891,33 @@
         <v>20</v>
       </c>
       <c r="G11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I11" s="2">
         <v>26</v>
       </c>
       <c r="J11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K11" t="s">
-        <v>36</v>
-      </c>
-      <c r="L11" t="s">
-        <v>37</v>
+        <v>35</v>
+      </c>
+      <c r="L11">
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B12">
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D12" s="2">
         <v>0</v>
@@ -929,33 +929,33 @@
         <v>10</v>
       </c>
       <c r="G12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I12" s="2">
         <v>20</v>
       </c>
       <c r="J12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K12" t="s">
-        <v>41</v>
-      </c>
-      <c r="L12" t="s">
-        <v>37</v>
+        <v>40</v>
+      </c>
+      <c r="L12">
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B13">
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D13" s="2">
         <v>0</v>
@@ -967,22 +967,22 @@
         <v>25</v>
       </c>
       <c r="G13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I13" s="2">
         <v>21</v>
       </c>
       <c r="J13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K13" t="s">
-        <v>36</v>
-      </c>
-      <c r="L13" t="s">
-        <v>37</v>
+        <v>35</v>
+      </c>
+      <c r="L13">
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -993,7 +993,7 @@
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D14" s="2">
         <v>0</v>
@@ -1005,33 +1005,33 @@
         <v>6</v>
       </c>
       <c r="G14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I14" s="2">
         <v>19</v>
       </c>
       <c r="J14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K14" t="s">
-        <v>36</v>
-      </c>
-      <c r="L14" t="s">
-        <v>37</v>
+        <v>35</v>
+      </c>
+      <c r="L14">
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B15">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D15" s="2">
         <v>0</v>
@@ -1043,33 +1043,33 @@
         <v>2</v>
       </c>
       <c r="G15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I15" s="2">
         <v>19</v>
       </c>
       <c r="J15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K15" t="s">
-        <v>40</v>
-      </c>
-      <c r="L15" t="s">
-        <v>37</v>
+        <v>39</v>
+      </c>
+      <c r="L15">
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B16">
         <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D16" s="2">
         <v>0</v>
@@ -1081,71 +1081,71 @@
         <v>2</v>
       </c>
       <c r="G16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I16" s="2">
         <v>25</v>
       </c>
       <c r="J16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K16" t="s">
-        <v>36</v>
-      </c>
-      <c r="L16" t="s">
-        <v>37</v>
+        <v>35</v>
+      </c>
+      <c r="L16">
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B17">
         <v>2</v>
       </c>
       <c r="C17" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" s="2">
+        <v>0</v>
+      </c>
+      <c r="E17" s="2">
+        <v>1</v>
+      </c>
+      <c r="F17" s="2">
+        <v>2</v>
+      </c>
+      <c r="G17" t="s">
+        <v>34</v>
+      </c>
+      <c r="H17" t="s">
         <v>37</v>
-      </c>
-      <c r="D17" s="2">
-        <v>0</v>
-      </c>
-      <c r="E17" s="2">
-        <v>1</v>
-      </c>
-      <c r="F17" s="2">
-        <v>2</v>
-      </c>
-      <c r="G17" t="s">
-        <v>35</v>
-      </c>
-      <c r="H17" t="s">
-        <v>38</v>
       </c>
       <c r="I17" s="2">
         <v>33</v>
       </c>
       <c r="J17" t="s">
+        <v>38</v>
+      </c>
+      <c r="K17" t="s">
         <v>39</v>
       </c>
-      <c r="K17" t="s">
-        <v>40</v>
-      </c>
-      <c r="L17" t="s">
-        <v>37</v>
+      <c r="L17">
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B18">
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D18" s="2">
         <v>0</v>
@@ -1157,33 +1157,33 @@
         <v>5</v>
       </c>
       <c r="G18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I18" s="2">
         <v>21</v>
       </c>
       <c r="J18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K18" t="s">
-        <v>36</v>
-      </c>
-      <c r="L18" t="s">
-        <v>37</v>
+        <v>35</v>
+      </c>
+      <c r="L18">
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B19">
         <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D19" s="2">
         <v>0</v>
@@ -1195,33 +1195,33 @@
         <v>13</v>
       </c>
       <c r="G19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I19" s="2">
         <v>38</v>
       </c>
       <c r="J19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K19" t="s">
-        <v>36</v>
-      </c>
-      <c r="L19" t="s">
-        <v>37</v>
+        <v>35</v>
+      </c>
+      <c r="L19">
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
       <c r="C20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D20" s="2">
         <v>0</v>
@@ -1233,33 +1233,33 @@
         <v>14</v>
       </c>
       <c r="G20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I20" s="2">
         <v>21</v>
       </c>
       <c r="J20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K20" t="s">
-        <v>36</v>
-      </c>
-      <c r="L20" t="s">
-        <v>37</v>
+        <v>35</v>
+      </c>
+      <c r="L20">
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B21">
         <v>1</v>
       </c>
       <c r="C21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D21" s="2">
         <v>0</v>
@@ -1271,33 +1271,33 @@
         <v>7</v>
       </c>
       <c r="G21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I21" s="2">
         <v>32</v>
       </c>
       <c r="J21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K21" t="s">
-        <v>36</v>
-      </c>
-      <c r="L21" t="s">
-        <v>39</v>
+        <v>35</v>
+      </c>
+      <c r="L21">
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B22">
         <v>2</v>
       </c>
       <c r="C22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D22" s="2">
         <v>0</v>
@@ -1309,22 +1309,22 @@
         <v>18</v>
       </c>
       <c r="G22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I22" s="2">
         <v>18</v>
       </c>
       <c r="J22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K22" t="s">
-        <v>36</v>
-      </c>
-      <c r="L22" t="s">
-        <v>39</v>
+        <v>35</v>
+      </c>
+      <c r="L22">
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -1335,80 +1335,83 @@
         <v>1</v>
       </c>
       <c r="C23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D23" s="2">
         <v>0</v>
       </c>
       <c r="E23" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F23" s="2">
         <v>4</v>
       </c>
       <c r="G23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I23" s="2">
         <v>18</v>
       </c>
       <c r="J23" t="s">
-        <v>37</v>
-      </c>
-      <c r="L23" t="s">
-        <v>39</v>
+        <v>36</v>
+      </c>
+      <c r="K23" t="s">
+        <v>35</v>
+      </c>
+      <c r="L23">
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B24">
         <v>2</v>
       </c>
       <c r="C24" t="s">
+        <v>36</v>
+      </c>
+      <c r="D24" s="2">
+        <v>0</v>
+      </c>
+      <c r="E24" s="2">
+        <v>1</v>
+      </c>
+      <c r="F24" s="2">
+        <v>2</v>
+      </c>
+      <c r="G24" t="s">
+        <v>34</v>
+      </c>
+      <c r="H24" t="s">
         <v>37</v>
-      </c>
-      <c r="D24" s="2">
-        <v>0</v>
-      </c>
-      <c r="E24" s="2">
-        <v>1</v>
-      </c>
-      <c r="F24" s="2">
-        <v>2</v>
-      </c>
-      <c r="G24" t="s">
-        <v>35</v>
-      </c>
-      <c r="H24" t="s">
-        <v>38</v>
       </c>
       <c r="I24" s="2">
         <v>18</v>
       </c>
       <c r="J24" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K24" t="s">
-        <v>36</v>
-      </c>
-      <c r="L24" t="s">
-        <v>39</v>
+        <v>35</v>
+      </c>
+      <c r="L24">
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B25">
         <v>2</v>
       </c>
       <c r="C25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D25" s="2">
         <v>0</v>
@@ -1420,54 +1423,60 @@
         <v>4</v>
       </c>
       <c r="G25" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H25" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I25" s="2">
         <v>21</v>
       </c>
       <c r="J25" t="s">
-        <v>39</v>
-      </c>
-      <c r="L25" t="s">
-        <v>39</v>
+        <v>38</v>
+      </c>
+      <c r="K25" t="s">
+        <v>35</v>
+      </c>
+      <c r="L25">
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B26">
         <v>1</v>
       </c>
       <c r="C26" t="s">
+        <v>36</v>
+      </c>
+      <c r="D26" s="2">
+        <v>0</v>
+      </c>
+      <c r="E26" s="2">
+        <v>2</v>
+      </c>
+      <c r="F26" s="2">
+        <v>3</v>
+      </c>
+      <c r="G26" t="s">
+        <v>34</v>
+      </c>
+      <c r="H26" t="s">
         <v>37</v>
-      </c>
-      <c r="D26" s="2">
-        <v>0</v>
-      </c>
-      <c r="E26" s="2">
-        <v>1</v>
-      </c>
-      <c r="F26" s="2">
-        <v>2</v>
-      </c>
-      <c r="G26" t="s">
-        <v>35</v>
-      </c>
-      <c r="H26" t="s">
-        <v>38</v>
       </c>
       <c r="I26" s="2">
         <v>20</v>
       </c>
       <c r="J26" t="s">
-        <v>37</v>
-      </c>
-      <c r="L26" t="s">
-        <v>39</v>
+        <v>36</v>
+      </c>
+      <c r="K26" t="s">
+        <v>35</v>
+      </c>
+      <c r="L26">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>